<commit_message>
benmap-46 removed number formatting
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -242,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -256,9 +256,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -268,17 +265,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -288,9 +275,23 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +428,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -521,11 +521,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="68085248"/>
-        <c:axId val="68086784"/>
+        <c:axId val="83937152"/>
+        <c:axId val="86036864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68085248"/>
+        <c:axId val="83937152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -535,7 +535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68086784"/>
+        <c:crossAx val="86036864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -543,7 +543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68086784"/>
+        <c:axId val="86036864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -574,7 +574,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
@@ -595,7 +594,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68085248"/>
+        <c:crossAx val="83937152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -622,7 +621,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -716,11 +714,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="89861504"/>
-        <c:axId val="89863296"/>
+        <c:axId val="86045440"/>
+        <c:axId val="86046976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89861504"/>
+        <c:axId val="86045440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -730,7 +728,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89863296"/>
+        <c:crossAx val="86046976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -738,7 +736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89863296"/>
+        <c:axId val="86046976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -749,14 +747,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89861504"/>
+        <c:crossAx val="86045440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1167,13 +1164,13 @@
   <dimension ref="A2:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D4" sqref="D4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="13" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="11" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="3"/>
     <col min="4" max="4" width="19.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" style="3" customWidth="1"/>
@@ -1196,16 +1193,16 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="20" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="22"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="15"/>
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -1253,16 +1250,16 @@
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -1289,34 +1286,34 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1335,69 +1332,68 @@
   <dimension ref="A2:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" style="14" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="18" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="3" customWidth="1"/>
-    <col min="5" max="10" width="10.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" style="21" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="22" customWidth="1"/>
+    <col min="5" max="10" width="10.7109375" style="22" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="22" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="15"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="23" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="4"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="1:11" ht="51.75" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="20" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="20" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
benmap-46 removed selected cells
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -266,22 +266,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -292,6 +280,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,11 +521,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="83937152"/>
-        <c:axId val="86036864"/>
+        <c:axId val="83936384"/>
+        <c:axId val="83937920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83937152"/>
+        <c:axId val="83936384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -535,7 +535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86036864"/>
+        <c:crossAx val="83937920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -543,7 +543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86036864"/>
+        <c:axId val="83937920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,7 +594,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83937152"/>
+        <c:crossAx val="83936384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -714,11 +714,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="86045440"/>
-        <c:axId val="86046976"/>
+        <c:axId val="88134016"/>
+        <c:axId val="88135552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86045440"/>
+        <c:axId val="88134016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -728,7 +728,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86046976"/>
+        <c:crossAx val="88135552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -736,7 +736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86046976"/>
+        <c:axId val="88135552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,7 +747,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86045440"/>
+        <c:crossAx val="88134016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1164,7 +1164,7 @@
   <dimension ref="A2:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:M4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -1193,16 +1193,16 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="13" t="s">
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="15"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="21"/>
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -1332,68 +1332,68 @@
   <dimension ref="A2:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1048576"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" style="21" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="22" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="22" customWidth="1"/>
-    <col min="5" max="10" width="10.7109375" style="22" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" style="22" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" style="17" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="18" customWidth="1"/>
+    <col min="5" max="10" width="10.7109375" style="18" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="18" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="17"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="14"/>
     </row>
     <row r="3" spans="1:11" ht="51.75" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="16" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrected summary chart to include only countries, no regions
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Detailed Results" sheetId="2" r:id="rId2"/>
     <sheet name="Avoided Deaths by country" sheetId="4" r:id="rId3"/>
     <sheet name="Avoided Deaths (% Population)" sheetId="5" r:id="rId4"/>
+    <sheet name="DataSource" sheetId="6" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -381,7 +382,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -475,11 +475,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="50131712"/>
-        <c:axId val="50133248"/>
+        <c:axId val="82004992"/>
+        <c:axId val="82019072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50131712"/>
+        <c:axId val="82004992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -489,7 +489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50133248"/>
+        <c:crossAx val="82019072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -497,7 +497,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50133248"/>
+        <c:axId val="82019072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,14 +520,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50131712"/>
+        <c:crossAx val="82004992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -662,11 +661,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="68199168"/>
-        <c:axId val="68235264"/>
+        <c:axId val="82037376"/>
+        <c:axId val="82055552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68199168"/>
+        <c:axId val="82037376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,7 +675,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68235264"/>
+        <c:crossAx val="82055552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -684,7 +683,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68235264"/>
+        <c:axId val="82055552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,7 +694,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68199168"/>
+        <c:crossAx val="82037376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1353,4 +1352,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added text box for total avoided deaths
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7530"/>
   </bookViews>
@@ -382,7 +382,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -476,11 +475,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82004608"/>
-        <c:axId val="82018688"/>
+        <c:axId val="82026880"/>
+        <c:axId val="82028416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82004608"/>
+        <c:axId val="82026880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,7 +489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82018688"/>
+        <c:crossAx val="82028416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -498,7 +497,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82018688"/>
+        <c:axId val="82028416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -521,14 +520,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82004608"/>
+        <c:crossAx val="82026880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -569,7 +567,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -663,11 +660,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82056704"/>
-        <c:axId val="82058624"/>
+        <c:axId val="90327680"/>
+        <c:axId val="90437120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82056704"/>
+        <c:axId val="90327680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -677,7 +674,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82058624"/>
+        <c:crossAx val="90437120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -685,7 +682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82058624"/>
+        <c:axId val="90437120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -696,7 +693,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82056704"/>
+        <c:crossAx val="90327680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -710,7 +707,7 @@
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
+  <sheetPr codeName="Chart3"/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -721,7 +718,7 @@
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
+  <sheetPr codeName="Chart4"/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -760,6 +757,65 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5362575" y="5314950"/>
+          <a:ext cx="4333875" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Avoided Deaths (Total):</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1106,11 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1273,6 +1328,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1353,6 +1409,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
benmap-142 populate ci, baseline mort, and deaths per 100,000
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -105,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,19 +129,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Gill Sans MT"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Gill Sans MT"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Gill Sans MT"/>
       <family val="2"/>
     </font>
@@ -294,10 +281,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -310,6 +293,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,11 +523,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="85155200"/>
-        <c:axId val="86492672"/>
+        <c:axId val="68029056"/>
+        <c:axId val="68030848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85155200"/>
+        <c:axId val="68029056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -550,7 +537,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86492672"/>
+        <c:crossAx val="68030848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -558,7 +545,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86492672"/>
+        <c:axId val="68030848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,7 +574,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85155200"/>
+        <c:crossAx val="68029056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -721,11 +708,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="87614976"/>
-        <c:axId val="87616512"/>
+        <c:axId val="68076672"/>
+        <c:axId val="68078208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87614976"/>
+        <c:axId val="68076672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -735,7 +722,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87616512"/>
+        <c:crossAx val="68078208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -743,7 +730,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87616512"/>
+        <c:axId val="68078208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -754,7 +741,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87614976"/>
+        <c:crossAx val="68076672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1226,8 +1213,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -1261,16 +1248,16 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="23" t="s">
+      <c r="K2" s="22"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="24"/>
-      <c r="O2" s="25"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="23"/>
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -1329,9 +1316,9 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -1441,16 +1428,16 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26" t="s">
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
       <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
benmap-142 center ci text
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -281,6 +281,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -293,10 +297,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,11 +523,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="68029056"/>
-        <c:axId val="68030848"/>
+        <c:axId val="89457792"/>
+        <c:axId val="89459328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68029056"/>
+        <c:axId val="89457792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -537,7 +537,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68030848"/>
+        <c:crossAx val="89459328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -545,7 +545,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68030848"/>
+        <c:axId val="89459328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -574,7 +574,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68029056"/>
+        <c:crossAx val="89457792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -708,11 +708,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="68076672"/>
-        <c:axId val="68078208"/>
+        <c:axId val="89432448"/>
+        <c:axId val="89433984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68076672"/>
+        <c:axId val="89432448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,7 +722,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68078208"/>
+        <c:crossAx val="89433984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -730,7 +730,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68078208"/>
+        <c:axId val="89433984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,7 +741,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68076672"/>
+        <c:crossAx val="89432448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1213,9 +1213,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1248,16 +1246,16 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="21" t="s">
+      <c r="K2" s="24"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="22"/>
-      <c r="O2" s="23"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="25"/>
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -1316,9 +1314,9 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -1428,16 +1426,16 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
       <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
benmap-142 calculate % baseline mortality at region and rollback level
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -281,10 +281,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -523,11 +523,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="89457792"/>
-        <c:axId val="89459328"/>
+        <c:axId val="79447552"/>
+        <c:axId val="101740928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89457792"/>
+        <c:axId val="79447552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -537,7 +537,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89459328"/>
+        <c:crossAx val="101740928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -545,7 +545,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89459328"/>
+        <c:axId val="101740928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -574,7 +574,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89457792"/>
+        <c:crossAx val="79447552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -708,11 +708,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="89432448"/>
-        <c:axId val="89433984"/>
+        <c:axId val="103956480"/>
+        <c:axId val="103958016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89432448"/>
+        <c:axId val="103956480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,7 +722,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89433984"/>
+        <c:crossAx val="103958016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -730,7 +730,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89433984"/>
+        <c:axId val="103958016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,7 +741,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89432448"/>
+        <c:crossAx val="103956480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1223,9 +1223,9 @@
     <col min="4" max="4" width="19.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="18.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="3" customWidth="1"/>
     <col min="8" max="8" width="13" style="3" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="3" customWidth="1"/>
     <col min="10" max="12" width="9.140625" style="3"/>
     <col min="13" max="13" width="9.7109375" style="3" customWidth="1"/>
     <col min="14" max="15" width="9.140625" style="3"/>
@@ -1314,9 +1314,9 @@
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -1401,7 +1401,7 @@
   <dimension ref="A2:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -1409,9 +1409,9 @@
     <col min="1" max="1" width="40.7109375" style="17" customWidth="1"/>
     <col min="2" max="3" width="20.7109375" style="18" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" style="18" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="18" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="18" customWidth="1"/>
     <col min="8" max="11" width="10.7109375" style="18" customWidth="1"/>
     <col min="12" max="13" width="9.140625" style="3"/>
     <col min="14" max="14" width="21.140625" style="3" customWidth="1"/>

</xml_diff>

<commit_message>
benmap-142 added metadata sheet
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7530"/>
+    <workbookView xWindow="4125" yWindow="1185" windowWidth="14370" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Detailed Results" sheetId="2" r:id="rId2"/>
     <sheet name="Avoided Deaths By Country" sheetId="4" r:id="rId3"/>
     <sheet name="Avoided Deaths (% Population)" sheetId="5" r:id="rId4"/>
-    <sheet name="DataSource" sheetId="6" state="hidden" r:id="rId5"/>
+    <sheet name="Metadata" sheetId="7" r:id="rId5"/>
+    <sheet name="DataSource" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -99,13 +100,547 @@
   </si>
   <si>
     <t>Deaths per 100,000</t>
+  </si>
+  <si>
+    <t>Supplementary Information / Underlying data and functions</t>
+  </si>
+  <si>
+    <r>
+      <t>A.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Air Quality Grid (PM2.5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description:  PM2.5 concentration data from the Global Burden of Disease 2010 study</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exposure Assessment for Estimation of the Global Burden of Disease Attributable to Outdoor Air Pollution</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Michael Brauer, Markus Amann, Rick T. Burnett, Aaron Cohen, Frank Dentener, Majid Ezzati, Sarah B. Henderson, Michal Krzyzanowski, Randall V. Martin, Rita Van Dingenen, Aaron van Donkelaar, and George D. Thurston</t>
+    </r>
+  </si>
+  <si>
+    <t>Environmental Science &amp; Technology 2012 46 (2), 652-660</t>
+  </si>
+  <si>
+    <r>
+      <t>B.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Population Grid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description:  Population data from 2010</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Center for International Earth Science Information Network: Gridded Population of the World, Version 3.0. Columbia University 2012</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Air Quality Standards</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description: Air Quality Standards / Guidelines / Objectives For Different Countries (updated April 2014).  Table developed by Scott Voorhees, US EPA.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Standards:</t>
+    </r>
+  </si>
+  <si>
+    <t>Standard Group</t>
+  </si>
+  <si>
+    <t>Concentration Limit</t>
+  </si>
+  <si>
+    <t>Exposure Duration</t>
+  </si>
+  <si>
+    <t>WHO</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>US Primary</t>
+  </si>
+  <si>
+    <t>US Secondary</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>China Class I</t>
+  </si>
+  <si>
+    <t>China Class II</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>24-hour</t>
+  </si>
+  <si>
+    <r>
+      <t>D.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Health Impact Function (Krewski et al, 2009)</t>
+    </r>
+  </si>
+  <si>
+    <t>a.       Reference: Krewski, D., M. Jerrett, R.T. Burnett, R. Ma, E. Hughes, et al. (2009). Extended Follow-Up and Spatial Analysis of the American Cancer Society Study Linking Particulate Air Pollution and Mortality. Health Effects Institute, Report Number 140. Cambridge, May.  http://pubs.healtheffects.org/getfile.php?u=478.</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>β = (Effective estimate) quantifies the change in health effects per unit of change in a pollutant and is derived from an epidemiological study</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ΔAQ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = change in pollutant concentration</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Incidence Rate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = baseline incident rate for the heath effect due to all causes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lim et al. A comparative risk assessment of burden of disease and injury attributable to 67 risk factors and risk factor clusters in 21 regions, 1990–2010: a systematic analysis for the Global Burden of Disease Study 2010, The Lancet, Volume 380, Issue 9859, 15 December 2012–4 January 2013, Pages 2224-2260, ISSN 0140-6736, http://dx.doi.org/10.1016/S0140-6736(12)61766-8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>File:  gbd_incrate_allcause_2010.csv</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Population</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Affected population</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>E.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Database</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Firebird database location: C:\ProgramData\BenMAP-CE\Database</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Firebird interface software: FlameRobin</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +667,38 @@
       <name val="Gill Sans MT"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -147,7 +714,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -235,11 +802,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -284,6 +900,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="13"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,6 +1092,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -523,11 +1186,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="79447552"/>
-        <c:axId val="101740928"/>
+        <c:axId val="91560576"/>
+        <c:axId val="91638784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79447552"/>
+        <c:axId val="91560576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -537,7 +1200,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101740928"/>
+        <c:crossAx val="91638784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -545,7 +1208,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101740928"/>
+        <c:axId val="91638784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -568,13 +1231,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79447552"/>
+        <c:crossAx val="91560576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -615,6 +1279,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -708,11 +1373,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="103956480"/>
-        <c:axId val="103958016"/>
+        <c:axId val="105329024"/>
+        <c:axId val="105330944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103956480"/>
+        <c:axId val="105329024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,7 +1387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103958016"/>
+        <c:crossAx val="105330944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -730,7 +1395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103958016"/>
+        <c:axId val="105330944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,7 +1406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103956480"/>
+        <c:crossAx val="105329024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -920,6 +1585,76 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="742950" y="6286500"/>
+          <a:ext cx="2705100" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1246,16 +1981,16 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="23" t="s">
+      <c r="K2" s="40"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="24"/>
-      <c r="O2" s="25"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="41"/>
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -1400,9 +2135,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1426,16 +2159,16 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26" t="s">
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
       <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1493,6 +2226,363 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="15" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="32">
+        <v>10</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="32">
+        <v>12</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="32">
+        <v>15</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="32">
+        <v>25</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="32">
+        <v>15</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="32">
+        <v>15</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="32">
+        <v>35</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="32">
+        <v>35</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="32">
+        <v>40</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="32">
+        <v>12</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="32">
+        <v>25</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="32">
+        <v>35</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="32">
+        <v>35</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="32">
+        <v>35</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="32">
+        <v>75</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="32">
+        <v>75</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="32">
+        <v>60</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="35">
+        <v>37.5</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="37"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1"/>

</xml_diff>

<commit_message>
benmap-142 updated metadata tab
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Detailed Results" sheetId="2" r:id="rId2"/>
     <sheet name="Avoided Deaths By Country" sheetId="4" r:id="rId3"/>
     <sheet name="Avoided Deaths (% Population)" sheetId="5" r:id="rId4"/>
-    <sheet name="Metadata" sheetId="7" r:id="rId5"/>
+    <sheet name="Metadata" sheetId="8" r:id="rId5"/>
     <sheet name="DataSource" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -105,56 +105,82 @@
     <t>Supplementary Information / Underlying data and functions</t>
   </si>
   <si>
+    <t>Standard Group</t>
+  </si>
+  <si>
+    <t>Concentration Limit</t>
+  </si>
+  <si>
+    <t>Exposure Duration</t>
+  </si>
+  <si>
+    <t>WHO</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>US Primary</t>
+  </si>
+  <si>
+    <t>US Secondary</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>China Class I</t>
+  </si>
+  <si>
+    <t>China Class II</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>24-hour</t>
+  </si>
+  <si>
+    <t>Air Quality Grid</t>
+  </si>
+  <si>
+    <t>Description:  PM2.5 concentration data from the Global Burden of Disease 2010 study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brauer, M.; Amann, M.; Burnett, R. T.; Cohen, A.; Dentener, F.; Ezzati, M.; Henderson, S. B.; Krzyzanowski, M.; Martin, R. V.; Van Dingenen, R.; van Donkelaar, A. &amp; Thurston, G. D. Exposure Assessment for Estimation of the Global Burden of Disease Attributable to Outdoor Air Pollution. Environ. Sci. Technol., Environmental Science &amp; Technology, American Chemical Society, 2011, 46, 652-660 </t>
+  </si>
+  <si>
+    <t>Population Grid</t>
+  </si>
+  <si>
+    <t>Description:  2010 Population Data</t>
+  </si>
+  <si>
+    <t>Center for International Earth Science Information Network: Gridded Population of the World, Version 3.0. Columbia University 2012</t>
+  </si>
+  <si>
+    <t>Health Impact Function (Krewski et al, 2009)</t>
+  </si>
+  <si>
+    <t>Krewski, D., M. Jerrett, R.T. Burnett, R. Ma, E. Hughes, et al. (2009). Extended Follow-Up and Spatial Analysis of the American Cancer Society Study Linking Particulate Air Pollution and Mortality. Health Effects Institute, Report Number 140. Cambridge, May.  http://pubs.healtheffects.org/getfile.php?u=478.</t>
+  </si>
+  <si>
     <r>
-      <t>A.</t>
+      <t>1.</t>
     </r>
     <r>
       <rPr>
         <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Air Quality Grid (PM2.5)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Description:  PM2.5 concentration data from the Global Burden of Disease 2010 study</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>b.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
@@ -163,255 +189,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Exposure Assessment for Estimation of the Global Burden of Disease Attributable to Outdoor Air Pollution</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>c.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Michael Brauer, Markus Amann, Rick T. Burnett, Aaron Cohen, Frank Dentener, Majid Ezzati, Sarah B. Henderson, Michal Krzyzanowski, Randall V. Martin, Rita Van Dingenen, Aaron van Donkelaar, and George D. Thurston</t>
-    </r>
-  </si>
-  <si>
-    <t>Environmental Science &amp; Technology 2012 46 (2), 652-660</t>
-  </si>
-  <si>
-    <r>
-      <t>B.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Population Grid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Description:  Population data from 2010</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>b.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Center for International Earth Science Information Network: Gridded Population of the World, Version 3.0. Columbia University 2012</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>C.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Air Quality Standards</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Description: Air Quality Standards / Guidelines / Objectives For Different Countries (updated April 2014).  Table developed by Scott Voorhees, US EPA.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>b.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Standards:</t>
-    </r>
-  </si>
-  <si>
-    <t>Standard Group</t>
-  </si>
-  <si>
-    <t>Concentration Limit</t>
-  </si>
-  <si>
-    <t>Exposure Duration</t>
-  </si>
-  <si>
-    <t>WHO</t>
-  </si>
-  <si>
-    <t>annual</t>
-  </si>
-  <si>
-    <t>US Primary</t>
-  </si>
-  <si>
-    <t>US Secondary</t>
-  </si>
-  <si>
-    <t>EU</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>China Class I</t>
-  </si>
-  <si>
-    <t>China Class II</t>
-  </si>
-  <si>
-    <t>Hong Kong</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>24-hour</t>
-  </si>
-  <si>
-    <r>
-      <t>D.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Health Impact Function (Krewski et al, 2009)</t>
-    </r>
-  </si>
-  <si>
-    <t>a.       Reference: Krewski, D., M. Jerrett, R.T. Burnett, R. Ma, E. Hughes, et al. (2009). Extended Follow-Up and Spatial Analysis of the American Cancer Society Study Linking Particulate Air Pollution and Mortality. Health Effects Institute, Report Number 140. Cambridge, May.  http://pubs.healtheffects.org/getfile.php?u=478.</t>
-  </si>
-  <si>
-    <r>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -426,6 +204,7 @@
     <r>
       <rPr>
         <sz val="7"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
@@ -435,6 +214,7 @@
       <rPr>
         <i/>
         <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -444,11 +224,12 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> = change in pollutant concentration</t>
+      <t xml:space="preserve"> = change in pollutant concentration (described above)</t>
     </r>
   </si>
   <si>
@@ -458,6 +239,7 @@
     <r>
       <rPr>
         <sz val="7"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
@@ -467,6 +249,7 @@
       <rPr>
         <i/>
         <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -476,171 +259,32 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> = baseline incident rate for the heath effect due to all causes</t>
+      <t xml:space="preserve"> = baseline incident rate for the heath effect due to all causes (comes from the specified database entry)</t>
     </r>
   </si>
   <si>
-    <r>
-      <t>a.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lim et al. A comparative risk assessment of burden of disease and injury attributable to 67 risk factors and risk factor clusters in 21 regions, 1990–2010: a systematic analysis for the Global Burden of Disease Study 2010, The Lancet, Volume 380, Issue 9859, 15 December 2012–4 January 2013, Pages 2224-2260, ISSN 0140-6736, http://dx.doi.org/10.1016/S0140-6736(12)61766-8</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>b.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>File:  gbd_incrate_allcause_2010.csv</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>4.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Population</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Affected population</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>E.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Database</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Firebird database location: C:\ProgramData\BenMAP-CE\Database</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>b.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Firebird interface software: FlameRobin</t>
-    </r>
+    <t>Reference: Lim et al. A comparative risk assessment of burden of disease and injury attributable to 67 risk factors and risk factor clusters in 21 regions, 1990–2010: a systematic analysis for the Global Burden of Disease Study 2010, The Lancet, Volume 380, Issue 9859, 15 December 2012–4 January 2013, Pages 2224-2260, ISSN 0140-6736, http://dx.doi.org/10.1016/S0140-6736(12)61766-8</t>
+  </si>
+  <si>
+    <t>Air Quality Standards</t>
+  </si>
+  <si>
+    <t>Description: Air Quality Standards / Guidelines / Objectives For Different Countries (updated April 2014).  Table developed by Scott Voorhees, US EPA.</t>
+  </si>
+  <si>
+    <t>Standards:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -670,31 +314,45 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="7"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <vertAlign val="superscript"/>
+      <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -714,7 +372,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -802,60 +460,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -901,52 +510,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="13"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -958,6 +521,28 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1186,11 +771,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="91560576"/>
-        <c:axId val="91638784"/>
+        <c:axId val="89654784"/>
+        <c:axId val="89656704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91560576"/>
+        <c:axId val="89654784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1200,7 +785,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91638784"/>
+        <c:crossAx val="89656704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1208,7 +793,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91638784"/>
+        <c:axId val="89656704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1238,7 +823,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91560576"/>
+        <c:crossAx val="89654784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1373,11 +958,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="105329024"/>
-        <c:axId val="105330944"/>
+        <c:axId val="79181696"/>
+        <c:axId val="79183232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="105329024"/>
+        <c:axId val="79181696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,7 +972,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105330944"/>
+        <c:crossAx val="79183232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1395,7 +980,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105330944"/>
+        <c:axId val="79183232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,7 +991,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105329024"/>
+        <c:crossAx val="79181696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1594,14 +1179,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2705100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1635,7 +1220,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="742950" y="6286500"/>
+          <a:off x="609600" y="3238500"/>
           <a:ext cx="2705100" cy="342900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1981,16 +1566,16 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="39" t="s">
+      <c r="J2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="39" t="s">
+      <c r="K2" s="24"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="40"/>
-      <c r="O2" s="41"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="25"/>
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -2159,16 +1744,16 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
       <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2230,355 +1815,309 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="15" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="24"/>
+    <col min="2" max="2" width="83.140625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="32">
-        <v>10</v>
-      </c>
-      <c r="D14" s="33" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="32">
-        <v>12</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="31" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="32">
-        <v>15</v>
-      </c>
-      <c r="D16" s="33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="32">
-        <v>25</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="32">
-        <v>15</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>43</v>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B16" s="28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="30" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="32">
-        <v>15</v>
-      </c>
-      <c r="D19" s="33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="32">
-        <v>35</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="32">
-        <v>35</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="32">
-        <v>40</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>43</v>
+      <c r="B19" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B21" s="30" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="32">
-        <v>12</v>
-      </c>
-      <c r="D23" s="33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="32">
-        <v>25</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="32">
-        <v>35</v>
-      </c>
-      <c r="D25" s="33" t="s">
-        <v>53</v>
+      <c r="A23" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="28" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="32">
-        <v>35</v>
-      </c>
-      <c r="D26" s="33" t="s">
-        <v>53</v>
+      <c r="B26" s="28" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="32">
+        <v>28</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="34">
+        <v>10</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="34">
+        <v>12</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="34">
+        <v>15</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="32">
+      <c r="C31" s="34">
+        <v>25</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="34">
+        <v>15</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="34">
+        <v>15</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="34">
+        <v>35</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="34">
+        <v>35</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="34">
+        <v>40</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="34">
+        <v>12</v>
+      </c>
+      <c r="D37" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="34">
+        <v>25</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="34">
+        <v>35</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="34">
+        <v>35</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="34">
+        <v>35</v>
+      </c>
+      <c r="D41" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="34">
         <v>75</v>
       </c>
-      <c r="D28" s="33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="32">
+      <c r="D42" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="34">
         <v>75</v>
       </c>
-      <c r="D29" s="33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="32">
+      <c r="D43" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="34">
         <v>60</v>
       </c>
-      <c r="D30" s="33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="35">
+      <c r="D44" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="34">
         <v>37.5</v>
       </c>
-      <c r="D31" s="36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="38"/>
+      <c r="D45" s="34" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
BF610 - updated metadata in rollback report
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmathews\Documents\RTI\Source\GitHub\benmap-ce\BenMAP\Tools\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="1185" windowWidth="14370" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -153,25 +158,47 @@
     <t>Air Quality Grid</t>
   </si>
   <si>
-    <t>Description:  PM2.5 concentration data from the Global Burden of Disease 2010 study</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brauer, M.; Amann, M.; Burnett, R. T.; Cohen, A.; Dentener, F.; Ezzati, M.; Henderson, S. B.; Krzyzanowski, M.; Martin, R. V.; Van Dingenen, R.; van Donkelaar, A. &amp; Thurston, G. D. Exposure Assessment for Estimation of the Global Burden of Disease Attributable to Outdoor Air Pollution. Environ. Sci. Technol., Environmental Science &amp; Technology, American Chemical Society, 2011, 46, 652-660 </t>
-  </si>
-  <si>
     <t>Population Grid</t>
   </si>
   <si>
-    <t>Description:  2010 Population Data</t>
-  </si>
-  <si>
-    <t>Center for International Earth Science Information Network: Gridded Population of the World, Version 3.0. Columbia University 2012</t>
-  </si>
-  <si>
     <t>Health Impact Function (Krewski et al, 2009)</t>
   </si>
   <si>
     <t>Krewski, D., M. Jerrett, R.T. Burnett, R. Ma, E. Hughes, et al. (2009). Extended Follow-Up and Spatial Analysis of the American Cancer Society Study Linking Particulate Air Pollution and Mortality. Health Effects Institute, Report Number 140. Cambridge, May.  http://pubs.healtheffects.org/getfile.php?u=478.</t>
+  </si>
+  <si>
+    <t>Air Quality Standards</t>
+  </si>
+  <si>
+    <t>Description: Air Quality Standards / Guidelines / Objectives For Different Countries (updated April 2014).  Table developed by Scott Voorhees, US EPA.</t>
+  </si>
+  <si>
+    <t>Standards:</t>
+  </si>
+  <si>
+    <t>Description:  PM2.5 concentration data from the Global Burden of Disease 2013 study</t>
+  </si>
+  <si>
+    <t>Description:  2015 Population Data</t>
+  </si>
+  <si>
+    <t>Center for International Earth Science Information Network - CIESIN - Columbia University. 2016. Gridded Population of the World, Version 4 (GPWv4): Administrative Unit Center Points with Population Estimates. Palisades, NY: NASA Socioeconomic Data and Applications Center (SEDAC). http://dx.doi.org/10.7927/H4F47M2C.</t>
+  </si>
+  <si>
+    <t>Incidence Dataset</t>
+  </si>
+  <si>
+    <t>Description: 2015 Cause-Specific Mortality</t>
+  </si>
+  <si>
+    <t>Global Burden of Disease Study 2015. Global Burden of Disease Study 2015 (GBD 2015) Life Expectancy, All-Cause and Cause-Specific Mortality 1980-2015. Seattle, United States: Institute for Health Metrics and Evaluation (IHME), 2016.
+http://ghdx.healthdata.org/record/global-burden-disease-study-2015-gbd-2015-life-expectancy-all-cause-and-cause-specific</t>
+  </si>
+  <si>
+    <t>Ambient Air Pollution Exposure Estimation for the Global Burden of Disease 2013
+Michael Brauer, Greg Freedman, Joseph Frostad, Aaron van Donkelaar, Randall V. Martin, Frank Dentener, Rita van Dingenen, Kara Estep, Heresh Amini, Joshua S. Apte, Kalpana Balakrishnan, Lars Barregard, David Broday, Valery Feigin, Santu Ghosh, Philip K. Hopke, Luke D. Knibbs, Yoshihiro Kokubo, Yang Liu, Stefan Ma, Lidia Morawska, José Luis Texcalac Sangrador, Gavin Shaddick, H. Ross Anderson, Theo Vos, Mohammad H. Forouzanfar, Richard T. Burnett, and Aaron Cohen.
+Environmental Science &amp; Technology 2016 50 (1), 79-88 
+DOI: 10.1021/acs.est.5b03709</t>
   </si>
   <si>
     <r>
@@ -180,7 +207,6 @@
     <r>
       <rPr>
         <sz val="7"/>
-        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
@@ -189,7 +215,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -204,7 +229,6 @@
     <r>
       <rPr>
         <sz val="7"/>
-        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
@@ -214,7 +238,6 @@
       <rPr>
         <i/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -224,7 +247,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -239,7 +261,6 @@
     <r>
       <rPr>
         <sz val="7"/>
-        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
@@ -249,7 +270,6 @@
       <rPr>
         <i/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -259,7 +279,6 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -267,24 +286,12 @@
       <t xml:space="preserve"> = baseline incident rate for the heath effect due to all causes (comes from the specified database entry)</t>
     </r>
   </si>
-  <si>
-    <t>Reference: Lim et al. A comparative risk assessment of burden of disease and injury attributable to 67 risk factors and risk factor clusters in 21 regions, 1990–2010: a systematic analysis for the Global Burden of Disease Study 2010, The Lancet, Volume 380, Issue 9859, 15 December 2012–4 January 2013, Pages 2224-2260, ISSN 0140-6736, http://dx.doi.org/10.1016/S0140-6736(12)61766-8</t>
-  </si>
-  <si>
-    <t>Air Quality Standards</t>
-  </si>
-  <si>
-    <t>Description: Air Quality Standards / Guidelines / Objectives For Different Countries (updated April 2014).  Table developed by Scott Voorhees, US EPA.</t>
-  </si>
-  <si>
-    <t>Standards:</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,9 +319,7 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -323,28 +328,6 @@
       <b/>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -352,7 +335,18 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -464,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -513,24 +507,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -543,6 +545,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,12 +568,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -588,7 +605,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -615,16 +631,9 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'Detailed Results'!#REF!</c:f>
-            </c:multiLvlStrRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Detailed Results'!#REF!</c:f>
@@ -637,6 +646,26 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Detailed Results'!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                  </c:multiLvlStrRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-21E9-4C8E-8CE2-574259B75E2D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -663,7 +692,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -677,7 +706,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -702,35 +730,6 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Detailed Results'!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>South Asia</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Aland</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Albania</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Algeria</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>American Samoa</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Andorra</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Angola</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Detailed Results'!#REF!</c:f>
@@ -761,6 +760,50 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Detailed Results'!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>South Asia</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Aland</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Albania</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Algeria</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>American Samoa</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Andorra</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Angola</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-670D-48F1-B870-0B3BA3CDF1E8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -816,7 +859,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
@@ -850,7 +892,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -884,7 +926,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -909,35 +950,6 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Detailed Results'!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>South Asia</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Aland</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Albania</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Algeria</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>American Samoa</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Andorra</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Angola</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Detailed Results'!#REF!</c:f>
@@ -968,6 +980,50 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Detailed Results'!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>South Asia</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Aland</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Albania</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Algeria</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>American Samoa</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Andorra</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Angola</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B595-4FD2-8708-848E74F2263B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1027,7 +1083,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart3"/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1038,7 +1094,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart4"/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1062,7 +1118,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2" title="By Country"/>
+        <xdr:cNvPr id="3" name="Chart 2" title="By Country">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1092,7 +1154,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1143,10 +1211,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8666963" cy="6297521"/>
+    <xdr:ext cx="8662051" cy="6293013"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
@@ -1170,10 +1244,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8666963" cy="6297521"/>
+    <xdr:ext cx="8662051" cy="6293013"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
@@ -1197,20 +1277,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2705100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1240,8 +1326,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="609600" y="3238500"/>
-          <a:ext cx="2705100" cy="342900"/>
+          <a:off x="609599" y="6229349"/>
+          <a:ext cx="2876551" cy="390525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1306,7 +1392,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1339,9 +1425,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1374,6 +1477,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1553,7 +1673,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1586,16 +1708,16 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="31" t="s">
+      <c r="K2" s="34"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="35"/>
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -1671,7 +1793,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>2010</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
@@ -1764,16 +1886,16 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34" t="s">
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
       <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1832,311 +1954,365 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="83.140625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="25" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="69.140625" style="25" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+    </row>
+    <row r="6" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+    </row>
+    <row r="11" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+    </row>
+    <row r="16" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+    <row r="22" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="38" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+    </row>
+    <row r="24" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+    </row>
+    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+    </row>
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
+    <row r="29" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="38" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="24" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B21" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="30">
-        <v>10</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="30">
-        <v>12</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="30">
-        <v>15</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="30">
-        <v>25</v>
-      </c>
-      <c r="D31" s="30" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="32">
+        <v>10</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="32">
+        <v>12</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="32">
+        <v>15</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="32">
+        <v>25</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="30">
+      <c r="C37" s="32">
         <v>15</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D37" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="29" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="30">
+      <c r="C38" s="32">
         <v>15</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D38" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="29" t="s">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="30">
+      <c r="C39" s="32">
         <v>35</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D39" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="29" t="s">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="30">
+      <c r="C40" s="32">
         <v>35</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D40" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="29" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="30">
+      <c r="C41" s="32">
         <v>40</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="D41" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="29" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="30">
+      <c r="C42" s="32">
         <v>12</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D42" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="29" t="s">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="30">
+      <c r="C43" s="32">
         <v>25</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D43" s="25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="29" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="30">
+      <c r="C44" s="32">
         <v>35</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D44" s="25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="29" t="s">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="30">
+      <c r="C45" s="32">
         <v>35</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D45" s="25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="29" t="s">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="30">
+      <c r="C46" s="32">
         <v>35</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D46" s="25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="29" t="s">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="30">
+      <c r="C47" s="32">
         <v>75</v>
       </c>
-      <c r="D42" s="30" t="s">
+      <c r="D47" s="25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="30">
+      <c r="C48" s="32">
         <v>75</v>
       </c>
-      <c r="D43" s="30" t="s">
+      <c r="D48" s="25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="30">
+      <c r="C49" s="32">
         <v>60</v>
       </c>
-      <c r="D44" s="30" t="s">
+      <c r="D49" s="25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="29" t="s">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="30">
+      <c r="C50" s="32">
         <v>37.5</v>
       </c>
-      <c r="D45" s="30" t="s">
+      <c r="D50" s="25" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="68" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
BF613 - updated metadata for incidence in rollback report
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -186,13 +186,6 @@
   </si>
   <si>
     <t>Incidence Dataset</t>
-  </si>
-  <si>
-    <t>Description: 2015 Cause-Specific Mortality</t>
-  </si>
-  <si>
-    <t>Global Burden of Disease Study 2015. Global Burden of Disease Study 2015 (GBD 2015) Life Expectancy, All-Cause and Cause-Specific Mortality 1980-2015. Seattle, United States: Institute for Health Metrics and Evaluation (IHME), 2016.
-http://ghdx.healthdata.org/record/global-burden-disease-study-2015-gbd-2015-life-expectancy-all-cause-and-cause-specific</t>
   </si>
   <si>
     <t>Ambient Air Pollution Exposure Estimation for the Global Burden of Disease 2013
@@ -285,6 +278,13 @@
       </rPr>
       <t xml:space="preserve"> = baseline incident rate for the heath effect due to all causes (comes from the specified database entry)</t>
     </r>
+  </si>
+  <si>
+    <t>Description: 2013 Cause-Specific Mortality</t>
+  </si>
+  <si>
+    <t>Global Burden of Disease Study 2013. Global Burden of Disease Study 2013 (GBD 2013) Incidence, Prevalence, and Years Lived with Disability 1990-2013. Seattle, United States: Institute for Health Metrics and Evaluation (IHME), 2015.
+http://ghdx.healthdata.org/record/global-burden-disease-study-2013-gbd-2013-incidence-prevalence-and-years-lived-disability</t>
   </si>
 </sst>
 </file>
@@ -546,17 +546,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1673,7 +1673,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1959,14 +1959,16 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" style="25" customWidth="1"/>
     <col min="2" max="2" width="23.140625" style="24" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="69.140625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="77.5703125" style="25" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
@@ -1981,19 +1983,19 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
     </row>
     <row r="6" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
-      <c r="B6" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
+      <c r="B6" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -2001,19 +2003,19 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
     </row>
     <row r="11" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
@@ -2021,22 +2023,22 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
+      <c r="B14" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
     </row>
     <row r="16" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
-      <c r="B16" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
+      <c r="B16" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -2044,32 +2046,32 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
     </row>
     <row r="24" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+    </row>
+    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+    </row>
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-    </row>
-    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-    </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
@@ -2077,11 +2079,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
@@ -2299,17 +2301,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="68" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
BF613- make summary page default in rollback report
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -546,17 +546,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1673,7 +1673,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1959,7 +1959,7 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1983,19 +1983,19 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
     </row>
     <row r="6" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -2003,19 +2003,19 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="11" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
@@ -2023,22 +2023,22 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
     </row>
     <row r="16" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -2046,32 +2046,32 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
     </row>
     <row r="24" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
     </row>
     <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
@@ -2079,11 +2079,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
@@ -2301,17 +2301,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="68" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
BF613- scroll metadata sheet to top
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -546,17 +546,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1083,7 +1083,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart3"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1094,7 +1094,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart4"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1211,7 +1211,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:ext cx="8670421" cy="6302523"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1244,7 +1244,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:ext cx="8670421" cy="6302523"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1673,7 +1673,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1959,7 +1959,7 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1983,19 +1983,19 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
     </row>
     <row r="6" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -2003,19 +2003,19 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
     </row>
     <row r="11" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
@@ -2023,22 +2023,22 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
     </row>
     <row r="16" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -2046,32 +2046,32 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
     </row>
     <row r="24" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
     </row>
     <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
@@ -2079,11 +2079,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
@@ -2301,17 +2301,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="68" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
BF613 summary default sheet
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -546,17 +546,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1673,7 +1673,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1959,7 +1959,7 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1983,19 +1983,19 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
     </row>
     <row r="6" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -2003,19 +2003,19 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="11" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
@@ -2023,22 +2023,22 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
     </row>
     <row r="16" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -2046,32 +2046,32 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
     </row>
     <row r="24" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
     </row>
     <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
@@ -2079,11 +2079,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
@@ -2301,17 +2301,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="68" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Release candidate build. Updated release notes and GBD Excel template
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmathews\Documents\RTI\Source\GitHub\benmap-ce\BenMAP\Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\benmap-ce\BenMAP\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -176,9 +176,6 @@
     <t>Standards:</t>
   </si>
   <si>
-    <t>Description:  PM2.5 concentration data from the Global Burden of Disease 2013 study</t>
-  </si>
-  <si>
     <t>Description:  2015 Population Data</t>
   </si>
   <si>
@@ -186,12 +183,6 @@
   </si>
   <si>
     <t>Incidence Dataset</t>
-  </si>
-  <si>
-    <t>Ambient Air Pollution Exposure Estimation for the Global Burden of Disease 2013
-Michael Brauer, Greg Freedman, Joseph Frostad, Aaron van Donkelaar, Randall V. Martin, Frank Dentener, Rita van Dingenen, Kara Estep, Heresh Amini, Joshua S. Apte, Kalpana Balakrishnan, Lars Barregard, David Broday, Valery Feigin, Santu Ghosh, Philip K. Hopke, Luke D. Knibbs, Yoshihiro Kokubo, Yang Liu, Stefan Ma, Lidia Morawska, José Luis Texcalac Sangrador, Gavin Shaddick, H. Ross Anderson, Theo Vos, Mohammad H. Forouzanfar, Richard T. Burnett, and Aaron Cohen.
-Environmental Science &amp; Technology 2016 50 (1), 79-88 
-DOI: 10.1021/acs.est.5b03709</t>
   </si>
   <si>
     <r>
@@ -285,6 +276,13 @@
   <si>
     <t>Global Burden of Disease Study 2013. Global Burden of Disease Study 2013 (GBD 2013) Incidence, Prevalence, and Years Lived with Disability 1990-2013. Seattle, United States: Institute for Health Metrics and Evaluation (IHME), 2015.
 http://ghdx.healthdata.org/record/global-burden-disease-study-2013-gbd-2013-incidence-prevalence-and-years-lived-disability</t>
+  </si>
+  <si>
+    <t>Description:  PM2.5 concentration data from the Global Burden of Disease 2015 study</t>
+  </si>
+  <si>
+    <t>Estimates and 25-year trends of the global burden of disease attributable to ambient air pollution: an analysis of data from the Global Burden of Diseases Study 2015
+Cohen, A. J.; Brauer, M.; Burnett, R. T. Lancet 2017, In press (17), 1–12.</t>
   </si>
 </sst>
 </file>
@@ -546,17 +544,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1083,7 +1081,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart3"/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="158" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1094,7 +1092,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart4"/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="158" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1211,7 +1209,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670421" cy="6302523"/>
+    <xdr:ext cx="8668956" cy="6293734"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1244,7 +1242,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670421" cy="6302523"/>
+    <xdr:ext cx="8668956" cy="6293734"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1673,8 +1671,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -1793,7 +1791,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>2013</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
@@ -1959,8 +1957,8 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1983,19 +1981,19 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-    </row>
-    <row r="6" spans="1:4" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+    </row>
+    <row r="6" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
-      <c r="B6" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
+      <c r="B6" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -2003,42 +2001,42 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
+      <c r="B9" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
     </row>
     <row r="11" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
-      <c r="B11" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
+      <c r="B11" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
+      <c r="B14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
     </row>
     <row r="16" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
-      <c r="B16" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
+      <c r="B16" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -2046,32 +2044,32 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
     </row>
     <row r="24" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+    </row>
+    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+    </row>
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-    </row>
-    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-    </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
@@ -2079,11 +2077,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
@@ -2301,17 +2299,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="68" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update GBD output Excel template. Add calculating YYL and Economic Benefit; Add function SCHIF and IER. Some issues need to be fixed.
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -1,30 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\benmap-ce\BenMAP\Tools\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="25200" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Detailed Results" sheetId="2" r:id="rId2"/>
     <sheet name="Avoided Deaths By Country" sheetId="4" r:id="rId3"/>
     <sheet name="Deaths Per 100,000" sheetId="5" r:id="rId4"/>
-    <sheet name="Metadata" sheetId="8" r:id="rId5"/>
-    <sheet name="DataSource" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet name="Economic Benefits" sheetId="10" r:id="rId5"/>
+    <sheet name="Metadata" sheetId="8" r:id="rId6"/>
+    <sheet name="DataSource" sheetId="6" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -284,11 +280,26 @@
     <t>Estimates and 25-year trends of the global burden of disease attributable to ambient air pollution: an analysis of data from the Global Burden of Diseases Study 2015
 Cohen, A. J.; Brauer, M.; Burnett, R. T. Lancet 2017, In press (17), 1–12.</t>
   </si>
+  <si>
+    <t>Economic Benefits</t>
+  </si>
+  <si>
+    <t>Avoided Life Years Lost</t>
+  </si>
+  <si>
+    <t>Change in Life Expectancy</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Value of Statistical Life Data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -456,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -532,6 +543,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -574,7 +586,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -603,6 +615,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -628,7 +641,7 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -644,7 +657,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
@@ -690,7 +703,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -758,7 +771,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
@@ -812,11 +825,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="89664512"/>
-        <c:axId val="94384896"/>
+        <c:axId val="101411456"/>
+        <c:axId val="113398144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89664512"/>
+        <c:axId val="101411456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -826,7 +839,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94384896"/>
+        <c:crossAx val="113398144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -834,7 +847,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94384896"/>
+        <c:axId val="113398144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -863,7 +876,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89664512"/>
+        <c:crossAx val="101411456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -890,7 +903,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -978,7 +991,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredCategoryTitle>
                 <c15:cat>
@@ -1032,11 +1045,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="94826880"/>
-        <c:axId val="94828416"/>
+        <c:axId val="113559040"/>
+        <c:axId val="113560576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="94826880"/>
+        <c:axId val="113559040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1046,7 +1059,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94828416"/>
+        <c:crossAx val="113560576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1054,7 +1067,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94828416"/>
+        <c:axId val="113560576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1065,7 +1078,195 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94826880"/>
+        <c:crossAx val="113559040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Economic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Benefits (USD)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Detailed Results'!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avoided Deaths (% Population)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Detailed Results'!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.72804187966218892</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25699347350814283</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33219052803782279</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5103699585040937</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0270301601888976</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.65306437227947778</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1095782351744758</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:filteredCategoryTitle>
+                <c15:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Detailed Results'!#REF!</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>South Asia</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Aland</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Albania</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Algeria</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>American Samoa</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Andorra</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Angola</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c15:cat>
+              </c15:filteredCategoryTitle>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B595-4FD2-8708-848E74F2263B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="113573248"/>
+        <c:axId val="114185344"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="113573248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="114185344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="114185344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113573248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1081,7 +1282,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart3"/>
   <sheetViews>
-    <sheetView zoomScale="158" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1092,7 +1293,18 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart4"/>
   <sheetViews>
-    <sheetView zoomScale="158" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1119,7 +1331,7 @@
         <xdr:cNvPr id="3" name="Chart 2" title="By Country">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1155,7 +1367,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1209,13 +1421,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668956" cy="6293734"/>
+    <xdr:ext cx="8658311" cy="6281351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1242,13 +1454,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668956" cy="6293734"/>
+    <xdr:ext cx="8658311" cy="6281351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1273,6 +1485,33 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8658311" cy="6281351"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1291,7 +1530,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1390,7 +1629,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1423,26 +1662,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1475,23 +1697,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1669,10 +1874,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:P14"/>
+  <dimension ref="A2:S14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -1685,15 +1890,15 @@
     <col min="6" max="6" width="18.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" style="3" customWidth="1"/>
     <col min="8" max="8" width="13" style="3" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="3" customWidth="1"/>
-    <col min="10" max="12" width="9.140625" style="3"/>
-    <col min="13" max="13" width="9.7109375" style="3" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="3"/>
-    <col min="16" max="16" width="21" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="3"/>
+    <col min="9" max="12" width="19.5703125" style="3" customWidth="1"/>
+    <col min="13" max="15" width="9.140625" style="3"/>
+    <col min="16" max="16" width="9.7109375" style="3" customWidth="1"/>
+    <col min="17" max="18" width="9.140625" style="3"/>
+    <col min="19" max="19" width="21" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1706,19 +1911,22 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="33" t="s">
+      <c r="N2" s="35"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q2" s="35"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1744,13 +1952,13 @@
         <v>9</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>10</v>
@@ -1762,10 +1970,19 @@
         <v>12</v>
       </c>
       <c r="P3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="51.75" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="51.75" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1785,8 +2002,11 @@
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1794,7 +2014,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1802,7 +2022,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1810,7 +2030,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1818,36 +2038,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="J2:L2"/>
     <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1858,9 +2082,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:N3"/>
+  <dimension ref="A2:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:M2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1869,14 +2095,14 @@
     <col min="4" max="4" width="18.85546875" style="18" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" style="18" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="18" customWidth="1"/>
-    <col min="8" max="11" width="10.7109375" style="18" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" style="3"/>
-    <col min="14" max="14" width="21.140625" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="10" width="19.5703125" style="18" customWidth="1"/>
+    <col min="11" max="14" width="10.7109375" style="18" customWidth="1"/>
+    <col min="15" max="16" width="9.140625" style="3"/>
+    <col min="17" max="17" width="21.140625" style="3" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="13"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -1884,19 +2110,22 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="14"/>
-    </row>
-    <row r="3" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="14"/>
+    </row>
+    <row r="3" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
@@ -1918,14 +2147,14 @@
       <c r="G3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>12</v>
+      <c r="H3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>10</v>
@@ -1937,13 +2166,22 @@
         <v>12</v>
       </c>
       <c r="N3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="16" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1957,7 +2195,7 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11:D11"/>
     </sheetView>
   </sheetViews>
@@ -1981,19 +2219,19 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="6" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -2001,19 +2239,19 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
     </row>
     <row r="11" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
@@ -2021,22 +2259,22 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
     </row>
     <row r="16" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -2044,32 +2282,32 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
     </row>
     <row r="24" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
     </row>
     <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
@@ -2077,11 +2315,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">

</xml_diff>

<commit_message>
Complete adding SCHIF and IER functions as well as YYL and Economic Benefits calculating. Some cleaning tasks remaining.
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="25200" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="25200" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>Value of Statistical Life Data</t>
+  </si>
+  <si>
+    <t>Economic Benefits (2011 USD)</t>
   </si>
 </sst>
 </file>
@@ -615,7 +618,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -825,11 +827,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="101411456"/>
-        <c:axId val="113398144"/>
+        <c:axId val="142858880"/>
+        <c:axId val="156102656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101411456"/>
+        <c:axId val="142858880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -839,7 +841,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113398144"/>
+        <c:crossAx val="156102656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -847,7 +849,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113398144"/>
+        <c:axId val="156102656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,7 +878,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101411456"/>
+        <c:crossAx val="142858880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1045,11 +1047,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="113559040"/>
-        <c:axId val="113560576"/>
+        <c:axId val="361780352"/>
+        <c:axId val="362184704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113559040"/>
+        <c:axId val="361780352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1059,7 +1061,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113560576"/>
+        <c:crossAx val="362184704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1067,7 +1069,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113560576"/>
+        <c:axId val="362184704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1080,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113559040"/>
+        <c:crossAx val="361780352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1233,11 +1235,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="113573248"/>
-        <c:axId val="114185344"/>
+        <c:axId val="142845440"/>
+        <c:axId val="142846976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="113573248"/>
+        <c:axId val="142845440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1247,7 +1249,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114185344"/>
+        <c:crossAx val="142846976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1255,7 +1257,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114185344"/>
+        <c:axId val="142846976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1266,7 +1268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113573248"/>
+        <c:crossAx val="142845440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1876,7 +1878,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -2084,8 +2086,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -2148,7 +2150,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Improve speed when calculating at grid cell level.
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="25200" windowHeight="11700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="25200" windowHeight="11700" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -279,9 +279,6 @@
   <si>
     <t>Estimates and 25-year trends of the global burden of disease attributable to ambient air pollution: an analysis of data from the Global Burden of Diseases Study 2015
 Cohen, A. J.; Brauer, M.; Burnett, R. T. Lancet 2017, In press (17), 1–12.</t>
-  </si>
-  <si>
-    <t>Economic Benefits</t>
   </si>
   <si>
     <t>Avoided Life Years Lost</t>
@@ -559,17 +556,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -618,6 +615,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -827,11 +825,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142858880"/>
-        <c:axId val="156102656"/>
+        <c:axId val="120848384"/>
+        <c:axId val="120850304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142858880"/>
+        <c:axId val="120848384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -841,7 +839,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156102656"/>
+        <c:crossAx val="120850304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -849,7 +847,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156102656"/>
+        <c:axId val="120850304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -878,7 +876,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142858880"/>
+        <c:crossAx val="120848384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1047,11 +1045,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="361780352"/>
-        <c:axId val="362184704"/>
+        <c:axId val="144358016"/>
+        <c:axId val="155566464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="361780352"/>
+        <c:axId val="144358016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1061,7 +1059,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="362184704"/>
+        <c:crossAx val="155566464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1069,7 +1067,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="362184704"/>
+        <c:axId val="155566464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1080,7 +1078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="361780352"/>
+        <c:crossAx val="144358016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1121,12 +1119,13 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Benefits (USD)</a:t>
+              <a:t> Benefits (2011 USD)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1235,11 +1234,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142845440"/>
-        <c:axId val="142846976"/>
+        <c:axId val="170084224"/>
+        <c:axId val="170085760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142845440"/>
+        <c:axId val="170084224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1249,7 +1248,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142846976"/>
+        <c:crossAx val="170085760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1257,7 +1256,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142846976"/>
+        <c:axId val="170085760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1268,7 +1267,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142845440"/>
+        <c:crossAx val="170084224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1306,7 +1305,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1333,7 +1332,7 @@
         <xdr:cNvPr id="3" name="Chart 2" title="By Country">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1369,7 +1368,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1429,7 +1428,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1462,7 +1461,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1489,7 +1488,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8658311" cy="6281351"/>
+    <xdr:ext cx="8662051" cy="6293013"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1532,7 +1531,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1878,8 +1877,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:S14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -1954,13 +1953,13 @@
         <v>9</v>
       </c>
       <c r="J3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>10</v>
@@ -2042,13 +2041,13 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="5"/>
     </row>
@@ -2086,8 +2085,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -2150,13 +2149,13 @@
         <v>9</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>61</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>62</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>10</v>
@@ -2221,19 +2220,19 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="6" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -2241,19 +2240,19 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
     </row>
     <row r="11" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
@@ -2261,22 +2260,22 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
     </row>
     <row r="16" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -2284,32 +2283,32 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
     </row>
     <row r="24" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
@@ -2317,11 +2316,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
@@ -2539,17 +2538,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="68" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correct Population weighted Air Quality data in final output.
</commit_message>
<xml_diff>
--- a/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
+++ b/BenMAP/Tools/GBDRollBackOutputTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="25200" windowHeight="11700" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="25200" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -556,17 +556,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -825,11 +825,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="120848384"/>
-        <c:axId val="120850304"/>
+        <c:axId val="170536320"/>
+        <c:axId val="170542208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="120848384"/>
+        <c:axId val="170536320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -839,7 +839,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120850304"/>
+        <c:crossAx val="170542208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -847,7 +847,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120850304"/>
+        <c:axId val="170542208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,7 +876,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120848384"/>
+        <c:crossAx val="170536320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1045,11 +1045,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144358016"/>
-        <c:axId val="155566464"/>
+        <c:axId val="189073664"/>
+        <c:axId val="189075456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144358016"/>
+        <c:axId val="189073664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1059,7 +1059,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155566464"/>
+        <c:crossAx val="189075456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1067,7 +1067,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="155566464"/>
+        <c:axId val="189075456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144358016"/>
+        <c:crossAx val="189073664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1234,11 +1234,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="170084224"/>
-        <c:axId val="170085760"/>
+        <c:axId val="189133184"/>
+        <c:axId val="189134720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170084224"/>
+        <c:axId val="189133184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,7 +1248,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170085760"/>
+        <c:crossAx val="189134720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1256,7 +1256,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170085760"/>
+        <c:axId val="189134720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1267,7 +1267,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170084224"/>
+        <c:crossAx val="189133184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1305,7 +1305,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="149" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1332,7 +1332,7 @@
         <xdr:cNvPr id="3" name="Chart 2" title="By Country">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1368,7 +1368,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1428,7 +1428,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1461,7 +1461,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1488,7 +1488,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:ext cx="8674782" cy="6296728"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1531,7 +1531,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1877,9 +1877,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:S14"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2220,19 +2218,19 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="6" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -2240,19 +2238,19 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
     </row>
     <row r="11" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
@@ -2260,22 +2258,22 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
     </row>
     <row r="16" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -2283,32 +2281,32 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
     </row>
     <row r="24" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
     </row>
     <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
@@ -2316,11 +2314,11 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
@@ -2538,17 +2536,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="68" orientation="portrait" r:id="rId1"/>

</xml_diff>